<commit_message>
fix dmx address dip decoding; reduce servo throw; create control document draft
</commit_message>
<xml_diff>
--- a/dmx control.xlsx
+++ b/dmx control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Beauty and the Beast\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F437A49-4DF8-47CF-A321-34FF151F1E29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D3D7B9-04FC-4BE2-A642-8DD38EE913D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B441C501-52AE-47C8-A241-77C0A6860D00}"/>
   </bookViews>
@@ -257,7 +257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -317,15 +317,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -429,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,22 +428,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -470,50 +461,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,7 +816,7 @@
   <dimension ref="B1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,61 +831,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="O1" s="16" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="25"/>
+      <c r="O1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="18"/>
-      <c r="U1" s="16" t="s">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="25"/>
+      <c r="U1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="18"/>
-      <c r="X1" s="25" t="s">
+      <c r="V1" s="25"/>
+      <c r="X1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
     </row>
     <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="24" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="21" t="s">
         <v>41</v>
       </c>
       <c r="O2" s="9" t="s">
@@ -924,23 +909,23 @@
       <c r="V2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="X2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="16" t="s">
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="24" t="s">
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -997,33 +982,33 @@
       <c r="V3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="19">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="24">
+      <c r="X3" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="21">
         <v>2</v>
       </c>
-      <c r="Z3" s="24">
+      <c r="Z3" s="21">
         <v>3</v>
       </c>
-      <c r="AA3" s="24">
+      <c r="AA3" s="21">
         <v>4</v>
       </c>
-      <c r="AB3" s="24">
+      <c r="AB3" s="21">
         <v>5</v>
       </c>
-      <c r="AC3" s="24" t="s">
+      <c r="AC3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" s="24" t="s">
+      <c r="AD3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AE3" s="24" t="s">
+      <c r="AE3" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1080,30 +1065,30 @@
       <c r="V4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="22">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="23" t="str">
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="20" t="str">
         <f>CONCATENATE(X4,Y4,Z4,AA4,AB4)</f>
         <v>00000</v>
       </c>
-      <c r="AD4" s="23">
+      <c r="AD4" s="20">
         <f>BIN2DEC(AC4)</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="23">
+      <c r="AE4" s="20">
         <f>AD4*16+1</f>
         <v>1</v>
       </c>
@@ -1130,19 +1115,19 @@
       <c r="V5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="X5" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="20">
+      <c r="X5" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="17">
         <v>1</v>
       </c>
       <c r="AC5" s="5" t="str">
@@ -1180,19 +1165,19 @@
       <c r="V6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="X6" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="20">
+      <c r="X6" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="17">
         <v>0</v>
       </c>
       <c r="AC6" s="5" t="str">
@@ -1232,19 +1217,19 @@
       <c r="S7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="20">
+      <c r="X7" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="17">
         <v>1</v>
       </c>
       <c r="AC7" s="5" t="str">
@@ -1283,19 +1268,19 @@
       <c r="S8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X8" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="20">
+      <c r="X8" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="17">
         <v>0</v>
       </c>
       <c r="AC8" s="5" t="str">
@@ -1334,19 +1319,19 @@
       <c r="S9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X9" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="20">
+      <c r="X9" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="17">
         <v>1</v>
       </c>
       <c r="AC9" s="5" t="str">
@@ -1385,19 +1370,19 @@
       <c r="S10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="20">
+      <c r="X10" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="17">
         <v>0</v>
       </c>
       <c r="AC10" s="5" t="str">
@@ -1436,19 +1421,19 @@
       <c r="S11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X11" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="20">
+      <c r="X11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="17">
         <v>1</v>
       </c>
       <c r="AC11" s="5" t="str">
@@ -1487,19 +1472,19 @@
       <c r="S12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="X12" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="20">
+      <c r="X12" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="17">
         <v>0</v>
       </c>
       <c r="AC12" s="5" t="str">
@@ -1538,19 +1523,19 @@
       <c r="S13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="X13" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="20">
+      <c r="X13" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="17">
         <v>1</v>
       </c>
       <c r="AC13" s="5" t="str">
@@ -1589,19 +1574,19 @@
       <c r="S14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X14" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="20">
+      <c r="X14" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="17">
         <v>0</v>
       </c>
       <c r="AC14" s="5" t="str">
@@ -1640,19 +1625,19 @@
       <c r="S15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="X15" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="20">
+      <c r="X15" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="17">
         <v>1</v>
       </c>
       <c r="AC15" s="5" t="str">
@@ -1691,19 +1676,19 @@
       <c r="S16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="X16" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="20">
+      <c r="X16" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="17">
         <v>0</v>
       </c>
       <c r="AC16" s="5" t="str">
@@ -1742,19 +1727,19 @@
       <c r="S17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="X17" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="20">
+      <c r="X17" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="17">
         <v>1</v>
       </c>
       <c r="AC17" s="5" t="str">
@@ -1793,19 +1778,19 @@
       <c r="S18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="X18" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB18" s="20">
+      <c r="X18" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="17">
         <v>0</v>
       </c>
       <c r="AC18" s="5" t="str">
@@ -1844,19 +1829,19 @@
       <c r="S19" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="X19" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="20">
+      <c r="X19" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="17">
         <v>1</v>
       </c>
       <c r="AC19" s="5" t="str">
@@ -1895,19 +1880,19 @@
       <c r="S20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="X20" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="20">
+      <c r="X20" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="17">
         <v>0</v>
       </c>
       <c r="AC20" s="5" t="str">
@@ -1946,19 +1931,19 @@
       <c r="S21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="X21" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="20">
+      <c r="X21" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="17">
         <v>1</v>
       </c>
       <c r="AC21" s="5" t="str">
@@ -1997,19 +1982,19 @@
       <c r="S22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="X22" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB22" s="20">
+      <c r="X22" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="17">
         <v>0</v>
       </c>
       <c r="AC22" s="5" t="str">
@@ -2048,19 +2033,19 @@
       <c r="S23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="X23" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="20">
+      <c r="X23" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="17">
         <v>1</v>
       </c>
       <c r="AC23" s="5" t="str">
@@ -2086,19 +2071,19 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="X24" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="20">
+      <c r="X24" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="17">
         <v>0</v>
       </c>
       <c r="AC24" s="5" t="str">
@@ -2126,19 +2111,19 @@
       <c r="N25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="X25" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="20">
+      <c r="X25" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="17">
         <v>1</v>
       </c>
       <c r="AC25" s="5" t="str">
@@ -2166,19 +2151,19 @@
       <c r="N26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="X26" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="20">
+      <c r="X26" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="17">
         <v>0</v>
       </c>
       <c r="AC26" s="5" t="str">
@@ -2206,19 +2191,19 @@
       <c r="N27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-      <c r="X27" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB27" s="20">
+      <c r="X27" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="17">
         <v>1</v>
       </c>
       <c r="AC27" s="5" t="str">
@@ -2246,19 +2231,19 @@
       <c r="N28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-      <c r="X28" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="20">
+      <c r="X28" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="17">
         <v>0</v>
       </c>
       <c r="AC28" s="5" t="str">
@@ -2278,19 +2263,19 @@
       <c r="G29" s="2"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-      <c r="X29" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="20">
+      <c r="X29" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="17">
         <v>1</v>
       </c>
       <c r="AC29" s="5" t="str">
@@ -2310,19 +2295,19 @@
       <c r="G30" s="2"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="X30" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="20">
+      <c r="X30" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="17">
         <v>0</v>
       </c>
       <c r="AC30" s="5" t="str">
@@ -2340,19 +2325,19 @@
     </row>
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G31" s="2"/>
-      <c r="X31" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z31" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB31" s="20">
+      <c r="X31" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="17">
         <v>1</v>
       </c>
       <c r="AC31" s="5" t="str">
@@ -2370,19 +2355,19 @@
     </row>
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G32" s="2"/>
-      <c r="X32" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y32" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z32" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="20">
+      <c r="X32" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="17">
         <v>0</v>
       </c>
       <c r="AC32" s="5" t="str">
@@ -2400,19 +2385,19 @@
     </row>
     <row r="33" spans="7:31" x14ac:dyDescent="0.25">
       <c r="G33" s="2"/>
-      <c r="X33" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z33" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="20">
+      <c r="X33" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="17">
         <v>1</v>
       </c>
       <c r="AC33" s="5" t="str">
@@ -2430,19 +2415,19 @@
     </row>
     <row r="34" spans="7:31" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
-      <c r="X34" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y34" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="20">
+      <c r="X34" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="17">
         <v>0</v>
       </c>
       <c r="AC34" s="5" t="str">
@@ -2460,19 +2445,19 @@
     </row>
     <row r="35" spans="7:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G35" s="2"/>
-      <c r="X35" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z35" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="21">
-        <v>1</v>
-      </c>
-      <c r="AB35" s="21">
+      <c r="X35" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="18">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="18">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="18">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="18">
         <v>1</v>
       </c>
       <c r="AC35" s="6" t="str">

</xml_diff>

<commit_message>
fix typo in control table
</commit_message>
<xml_diff>
--- a/dmx control.xlsx
+++ b/dmx control.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Beauty and the Beast\arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Beauty and the Beast\Rose\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD48D693-AA84-4E22-A69B-615A99D89F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018DAFB5-0EEE-4A42-8D4B-0640FCDA8507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="2115" windowWidth="21345" windowHeight="13125" xr2:uid="{B441C501-52AE-47C8-A241-77C0A6860D00}"/>
+    <workbookView xWindow="2625" yWindow="2625" windowWidth="21345" windowHeight="13125" xr2:uid="{B441C501-52AE-47C8-A241-77C0A6860D00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -997,15 +997,17 @@
   <dimension ref="B1:AE37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="O2" sqref="O2:S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="10.28515625" customWidth="1"/>
-    <col min="15" max="18" width="10.42578125" customWidth="1"/>
-    <col min="19" max="19" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.42578125" customWidth="1"/>
+    <col min="19" max="19" width="58.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -2254,7 +2256,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="22">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="P25" s="23" t="s">
         <v>18</v>
@@ -2307,7 +2309,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="25">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="P26" s="26" t="s">
         <v>18</v>
@@ -2360,7 +2362,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="25">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="P27" s="26" t="s">
         <v>18</v>
@@ -2413,7 +2415,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="25">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="P28" s="26" t="s">
         <v>18</v>
@@ -2466,7 +2468,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="25">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="P29" s="26" t="s">
         <v>18</v>
@@ -2511,7 +2513,7 @@
     <row r="30" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="2"/>
       <c r="O30" s="17">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="P30" s="18" t="s">
         <v>18</v>
@@ -2556,7 +2558,7 @@
     <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G31" s="2"/>
       <c r="O31" s="22">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="P31" s="23" t="s">
         <v>18</v>
@@ -2601,7 +2603,7 @@
     <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G32" s="2"/>
       <c r="O32" s="25">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="P32" s="26" t="s">
         <v>18</v>
@@ -2646,7 +2648,7 @@
     <row r="33" spans="7:31" x14ac:dyDescent="0.25">
       <c r="G33" s="2"/>
       <c r="O33" s="25">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="P33" s="26" t="s">
         <v>18</v>
@@ -2691,7 +2693,7 @@
     <row r="34" spans="7:31" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
       <c r="O34" s="25">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="P34" s="26" t="s">
         <v>18</v>
@@ -2736,7 +2738,7 @@
     <row r="35" spans="7:31" x14ac:dyDescent="0.25">
       <c r="G35" s="2"/>
       <c r="O35" s="25">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="P35" s="26" t="s">
         <v>18</v>
@@ -2781,7 +2783,7 @@
     <row r="36" spans="7:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G36" s="2"/>
       <c r="O36" s="17">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="P36" s="18" t="s">
         <v>18</v>

</xml_diff>